<commit_message>
updated sampleTable.xlsx (rownames to colum)
</commit_message>
<xml_diff>
--- a/data/processed/sampleTable.xlsx
+++ b/data/processed/sampleTable.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,6 +360,11 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Sample</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>group</t>
         </is>
       </c>
@@ -367,6 +372,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>SRR11856091</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>baseline</t>
         </is>
       </c>
@@ -374,6 +384,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>SRR11856092</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>baseline</t>
         </is>
       </c>
@@ -381,6 +396,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>SRR11856093</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>baseline</t>
         </is>
       </c>
@@ -388,6 +408,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>SRR11856094</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>3 weeks RMPI</t>
         </is>
       </c>
@@ -395,6 +420,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>SRR11856095</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>3 weeks RMPI</t>
         </is>
       </c>
@@ -402,6 +432,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>SRR11856096</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>3 weeks RMPI</t>
         </is>
       </c>
@@ -409,6 +444,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>SRR11856097</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>3 weeks MM</t>
         </is>
       </c>
@@ -416,6 +456,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>SRR11856098</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>3 weeks MM</t>
         </is>
       </c>
@@ -423,12 +468,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>SRR11856099</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>3 weeks MM</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
+        <is>
+          <t>SRR11856100</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>3 weeks MM</t>
         </is>

</xml_diff>

<commit_message>
update files to new dataset
</commit_message>
<xml_diff>
--- a/data/processed/sampleTable.xlsx
+++ b/data/processed/sampleTable.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,6 +365,16 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>temperature</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>treatment</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>group</t>
         </is>
       </c>
@@ -372,120 +382,264 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SRR11856091</t>
+          <t>SRR10908157</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>baseline</t>
+          <t>35C</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>DMSO</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>35C_DMSO</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SRR11856092</t>
+          <t>SRR10908158</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>baseline</t>
+          <t>35C</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>DMSO</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>35C_DMSO</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SRR11856093</t>
+          <t>SRR10908159</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>baseline</t>
+          <t>35C</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>DMSO</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>35C_DMSO</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SRR11856094</t>
+          <t>SRR10908160</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3 weeks RMPI</t>
+          <t>35C</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>TG003</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>35C_TG003</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SRR11856095</t>
+          <t>SRR10908161</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3 weeks RMPI</t>
+          <t>35C</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>TG003</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>35C_TG003</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SRR11856096</t>
+          <t>SRR10908162</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>3 weeks RMPI</t>
+          <t>35C</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>TG003</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>35C_TG003</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SRR11856097</t>
+          <t>SRR10908163</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>3 weeks MM</t>
+          <t>39C</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>DMSO</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>39C_DMSO</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SRR11856098</t>
+          <t>SRR10908164</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3 weeks MM</t>
+          <t>39C</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>DMSO</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>39C_DMSO</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>SRR11856099</t>
+          <t>SRR10908165</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3 weeks MM</t>
+          <t>39C</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>DMSO</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>39C_DMSO</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SRR11856100</t>
+          <t>SRR10908166</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3 weeks MM</t>
+          <t>39C</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>TG003</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>39C_TG003</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SRR10908167</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>39C</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>TG003</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>39C_TG003</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>SRR10908168</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>39C</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>TG003</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>39C_TG003</t>
         </is>
       </c>
     </row>

</xml_diff>